<commit_message>
Updated list for names.
</commit_message>
<xml_diff>
--- a/Used_names_list.xlsx
+++ b/Used_names_list.xlsx
@@ -96,18 +96,12 @@
     <t>a matrix that contains the occurrence points of a species and the environmental data of the find location</t>
   </si>
   <si>
-    <t>species</t>
-  </si>
-  <si>
     <t>ranpoints</t>
   </si>
   <si>
     <t>M.shp, shp</t>
   </si>
   <si>
-    <t>save.map, save.p</t>
-  </si>
-  <si>
     <t>cloud</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>sample size</t>
+  </si>
+  <si>
+    <t>save.p</t>
+  </si>
+  <si>
+    <t>species, occ</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -596,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -607,7 +607,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -615,26 +615,26 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>